<commit_message>
Commit for Change in Title name from Login Page
Commit for Change in Title name from Login Page
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pushk\git\repository\Selenium_Framework\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C632B632-C626-48ED-829B-043352E6D932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E33F257-1407-4466-B918-9788D6CB554B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Username</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>vidya.bhadang@gmail.com</t>
-  </si>
-  <si>
-    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -110,9 +107,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -396,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,35 +405,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -446,7 +434,6 @@
     <hyperlink ref="B2" r:id="rId2" xr:uid="{3820A672-C218-40C1-972D-D29FB42287AE}"/>
     <hyperlink ref="A3" r:id="rId3" xr:uid="{72580614-606A-43FE-8DEF-BD678DB2FB1A}"/>
     <hyperlink ref="B3" r:id="rId4" xr:uid="{A40E0682-E42E-452E-B960-CF1462EB5555}"/>
-    <hyperlink ref="A4" r:id="rId5" xr:uid="{38AB1409-A978-4B77-941F-3B45AA6C13EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update README with installation instructions
Added a new section to the README file detailing the steps required to install project dependencies and set up the development environment.
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pushk\git\repository\Selenium_Framework\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E33F257-1407-4466-B918-9788D6CB554B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBE2FB5-86D3-41B7-8B2D-6DE3039BCEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Username</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>vidya.bhadang@gmail.com</t>
+  </si>
+  <si>
+    <t>Test@123</t>
   </si>
 </sst>
 </file>
@@ -395,7 +398,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,7 +428,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update TestData.xlsx with new test data
The TestData.xlsx file in the testdata directory has been updated. This may include new or modified test cases to support recent changes or improvements in testing coverage.
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pushk\git\repository\Selenium_Framework\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBE2FB5-86D3-41B7-8B2D-6DE3039BCEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD902A42-E053-419F-9A2B-881FE7FE9CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Username</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>vidya.bhadang@gmail.com</t>
-  </si>
-  <si>
-    <t>Test@123</t>
   </si>
 </sst>
 </file>
@@ -398,7 +395,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,7 +425,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -436,7 +433,7 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{0E358D82-EA7E-4797-98B4-EAB5C067563B}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{3820A672-C218-40C1-972D-D29FB42287AE}"/>
     <hyperlink ref="A3" r:id="rId3" xr:uid="{72580614-606A-43FE-8DEF-BD678DB2FB1A}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{A40E0682-E42E-452E-B960-CF1462EB5555}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{ACA9338C-F67A-4C5F-8A74-8894C87E715C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>